<commit_message>
Backlog del producto terminado
</commit_message>
<xml_diff>
--- a/01. INICIO/Backlog del Producto.xlsx
+++ b/01. INICIO/Backlog del Producto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13710" windowHeight="5895" tabRatio="522"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="522"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog del Producto" sheetId="8" r:id="rId1"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
   <si>
     <t>Sprint</t>
   </si>
@@ -368,6 +368,57 @@
   </si>
   <si>
     <t xml:space="preserve">Debe poder mostrar los procesos de las funcionalidades del sistema </t>
+  </si>
+  <si>
+    <t>Debe poder almacenar la informacion</t>
+  </si>
+  <si>
+    <t>Deber poder mostrar el esquema de la ventana</t>
+  </si>
+  <si>
+    <t>Debe poder mostrar la funcionalidad del sistema</t>
+  </si>
+  <si>
+    <t>Entrega del software</t>
+  </si>
+  <si>
+    <t>pruebas del software</t>
+  </si>
+  <si>
+    <t>deseo facturacion</t>
+  </si>
+  <si>
+    <t>deseo control de sucursales</t>
+  </si>
+  <si>
+    <t>deseo contro de stock</t>
+  </si>
+  <si>
+    <t>HU07</t>
+  </si>
+  <si>
+    <t>HU08</t>
+  </si>
+  <si>
+    <t>HU09</t>
+  </si>
+  <si>
+    <t>Presentar los comprobaste de las ventas</t>
+  </si>
+  <si>
+    <t>Presentar el control de stock de los almacenes de la  tienda</t>
+  </si>
+  <si>
+    <t>Presentar el manejo de las diferentes sucursales</t>
+  </si>
+  <si>
+    <t>debe emitir los comprabantes de las ventas realizadas y manejo de crud</t>
+  </si>
+  <si>
+    <t>debe emitir los diferentes reportes de las ventas por sucursal y manejo de crud</t>
+  </si>
+  <si>
+    <t>debe emitir los reportes del stock de los diferentes almacenes y manejo de crud</t>
   </si>
 </sst>
 </file>
@@ -562,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -684,6 +735,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -717,8 +771,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1300,7 +1363,7 @@
   <dimension ref="B1:S80"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1337,14 +1400,14 @@
       </c>
     </row>
     <row r="2" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="56"/>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -1363,14 +1426,14 @@
       </c>
     </row>
     <row r="3" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="55"/>
+      <c r="E3" s="56"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -1411,27 +1474,27 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51" t="s">
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="54"/>
     </row>
     <row r="6" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="34" t="s">
@@ -1531,7 +1594,7 @@
       <c r="L8" s="8">
         <v>30</v>
       </c>
-      <c r="M8" s="56" t="s">
+      <c r="M8" s="45" t="s">
         <v>31</v>
       </c>
       <c r="N8" s="8">
@@ -1568,7 +1631,7 @@
       <c r="L9" s="8">
         <v>40</v>
       </c>
-      <c r="M9" s="56" t="s">
+      <c r="M9" s="45" t="s">
         <v>32</v>
       </c>
       <c r="N9" s="8">
@@ -1605,7 +1668,7 @@
       <c r="L10" s="8">
         <v>25</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="45" t="s">
         <v>33</v>
       </c>
       <c r="N10" s="8">
@@ -1658,14 +1721,16 @@
       <c r="I12" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="K12" s="8">
         <v>1</v>
       </c>
       <c r="L12" s="8">
         <v>40</v>
       </c>
-      <c r="M12" s="56" t="s">
+      <c r="M12" s="45" t="s">
         <v>34</v>
       </c>
       <c r="N12" s="8">
@@ -1693,14 +1758,16 @@
       <c r="I13" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="25" t="s">
+        <v>65</v>
+      </c>
       <c r="K13" s="8">
         <v>1</v>
       </c>
       <c r="L13" s="8">
         <v>40</v>
       </c>
-      <c r="M13" s="56" t="s">
+      <c r="M13" s="45" t="s">
         <v>48</v>
       </c>
       <c r="N13" s="8">
@@ -1728,14 +1795,16 @@
       <c r="I14" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="25" t="s">
+        <v>66</v>
+      </c>
       <c r="K14" s="8">
         <v>1</v>
       </c>
       <c r="L14" s="8">
         <v>40</v>
       </c>
-      <c r="M14" s="56" t="s">
+      <c r="M14" s="45" t="s">
         <v>49</v>
       </c>
       <c r="N14" s="8">
@@ -1750,12 +1819,18 @@
       <c r="B15" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+      <c r="C15" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>68</v>
+      </c>
       <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="43"/>
       <c r="J15" s="9"/>
       <c r="K15" s="8"/>
@@ -1765,55 +1840,115 @@
       <c r="O15" s="8"/>
       <c r="P15" s="9"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B16" s="43"/>
       <c r="C16" s="43"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="F16" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>10</v>
+      </c>
+      <c r="M16" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="8">
+        <v>7</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="P16" s="9"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B17" s="43"/>
       <c r="C17" s="43"/>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
+      <c r="F17" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1</v>
+      </c>
+      <c r="L17" s="8">
+        <v>10</v>
+      </c>
+      <c r="M17" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="N17" s="8">
+        <v>8</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="P17" s="9"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B18" s="43"/>
       <c r="C18" s="43"/>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="F18" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1</v>
+      </c>
+      <c r="L18" s="8">
+        <v>10</v>
+      </c>
+      <c r="M18" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="N18" s="8">
+        <v>9</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="P18" s="9"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
@@ -2446,7 +2581,7 @@
       <formula>$O70="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:G7 I7 K7:P125 B8:J125">
+  <conditionalFormatting sqref="B7:G7 I7 B8:J125 K7:P125">
     <cfRule type="expression" dxfId="15" priority="31" stopIfTrue="1">
       <formula>$O7="Terminado"</formula>
     </cfRule>
@@ -2500,7 +2635,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2694,92 +2829,92 @@
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="17" t="str">
-        <f t="shared" ref="B9:B17" si="2">IF(AND(C9&lt;&gt;"",D9&lt;&gt;""),B8+1,"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="19" t="str">
-        <f t="shared" ref="C9:C17" si="3">IF(AND(C8&lt;&gt;"",D8&lt;&gt;"",D9&lt;&gt;""),C8+D8,"")</f>
-        <v/>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21" t="str">
-        <f t="shared" ref="E9:E17" si="4">IF(AND(C9&lt;&gt;"",D9&lt;&gt;""),C9+D9-1,"")</f>
-        <v/>
-      </c>
-      <c r="F9" s="17" t="str">
+      <c r="B9" s="57">
+        <v>7</v>
+      </c>
+      <c r="C9" s="58">
+        <f t="shared" ref="C9:C17" si="2">IF(AND(C8&lt;&gt;"",D8&lt;&gt;"",D9&lt;&gt;""),C8+D8,"")</f>
+        <v>45048</v>
+      </c>
+      <c r="D9" s="59">
+        <v>2</v>
+      </c>
+      <c r="E9" s="60">
+        <f t="shared" ref="E9:E17" si="3">IF(AND(C9&lt;&gt;"",D9&lt;&gt;""),C9+D9-1,"")</f>
+        <v>45049</v>
+      </c>
+      <c r="F9" s="57">
         <f>IF(B9="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B9,'Backlog del Producto'!L$8:L$130))</f>
-        <v/>
-      </c>
-      <c r="G9" s="18" t="str">
-        <f t="shared" ref="G9:G17" si="5">IF(AND(OR(G8="Planned",G8="Ongoing"),D9&lt;&gt;""),"Planned","Unplanned")</f>
-        <v>Unplanned</v>
+        <v>10</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="str">
+      <c r="B10" s="57">
+        <v>8</v>
+      </c>
+      <c r="C10" s="58">
+        <f t="shared" si="2"/>
+        <v>45050</v>
+      </c>
+      <c r="D10" s="59">
+        <v>2</v>
+      </c>
+      <c r="E10" s="60">
+        <f t="shared" si="3"/>
+        <v>45051</v>
+      </c>
+      <c r="F10" s="57">
+        <f>IF(B10="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B10,'Backlog del Producto'!L$8:L$130))</f>
+        <v>10</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="57">
+        <v>9</v>
+      </c>
+      <c r="C11" s="58">
+        <f t="shared" si="2"/>
+        <v>45052</v>
+      </c>
+      <c r="D11" s="59">
+        <v>2</v>
+      </c>
+      <c r="E11" s="60">
+        <f t="shared" si="3"/>
+        <v>45053</v>
+      </c>
+      <c r="F11" s="57">
+        <f>IF(B11="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B11,'Backlog del Producto'!L$8:L$130))</f>
+        <v>10</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="17" t="str">
+        <f t="shared" ref="B9:B17" si="4">IF(AND(C12&lt;&gt;"",D12&lt;&gt;""),B11+1,"")</f>
+        <v/>
+      </c>
+      <c r="C12" s="19" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C10" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F10" s="17" t="str">
-        <f>IF(B10="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B10,'Backlog del Producto'!L$8:L$130))</f>
-        <v/>
-      </c>
-      <c r="G10" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>Unplanned</v>
-      </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C11" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="F11" s="17" t="str">
-        <f>IF(B11="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B11,'Backlog del Producto'!L$8:L$130))</f>
-        <v/>
-      </c>
-      <c r="G11" s="18" t="str">
-        <f t="shared" si="5"/>
-        <v>Unplanned</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C12" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="D12" s="20"/>
       <c r="E12" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F12" s="17" t="str">
@@ -2787,7 +2922,7 @@
         <v/>
       </c>
       <c r="G12" s="18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="G9:G17" si="5">IF(AND(OR(G11="Planned",G11="Ongoing"),D12&lt;&gt;""),"Planned","Unplanned")</f>
         <v>Unplanned</v>
       </c>
       <c r="H12" s="20"/>
@@ -2795,16 +2930,16 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C13" s="19" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C13" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="D13" s="20"/>
       <c r="E13" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F13" s="17" t="str">
@@ -2820,16 +2955,16 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C14" s="19" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C14" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F14" s="17" t="str">
@@ -2845,16 +2980,16 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C15" s="19" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C15" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F15" s="17" t="str">
@@ -2870,16 +3005,16 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C16" s="19" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C16" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F16" s="17" t="str">
@@ -2895,16 +3030,16 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C17" s="19" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C17" s="19" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F17" s="17" t="str">
@@ -2974,6 +3109,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3245187f-2b70-4b96-af74-b65b25777eca" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="100486ed-dfc5-4b43-a390-ed80e6fa3473">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ECBD21C84E4C4B48B27A6166FAC051E5" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="bb6739421a50b20a8dee76844e41c5f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="100486ed-dfc5-4b43-a390-ed80e6fa3473" xmlns:ns3="3245187f-2b70-4b96-af74-b65b25777eca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="093860096c687094a446cbcfc6e32844" ns2:_="" ns3:_="">
     <xsd:import namespace="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
@@ -3150,58 +3309,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3245187f-2b70-4b96-af74-b65b25777eca" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="100486ed-dfc5-4b43-a390-ed80e6fa3473">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B83DAEE-35DE-44AA-B387-4AFD3E8AB467}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
-    <ds:schemaRef ds:uri="3245187f-2b70-4b96-af74-b65b25777eca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3219,10 +3335,29 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B83DAEE-35DE-44AA-B387-4AFD3E8AB467}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
+    <ds:schemaRef ds:uri="3245187f-2b70-4b96-af74-b65b25777eca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Backlog Detallado del producto terminado
</commit_message>
<xml_diff>
--- a/01. INICIO/Backlog del Producto.xlsx
+++ b/01. INICIO/Backlog del Producto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="522"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10530" windowHeight="7320" tabRatio="522"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog del Producto" sheetId="8" r:id="rId1"/>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
   <si>
     <t>Sprint</t>
   </si>
@@ -343,9 +343,6 @@
     <t>Presentar los diferentes diagramas de BMP</t>
   </si>
   <si>
-    <t>Debe poder mostrar los procesos de las funcionalidades del proceso Debe poderse filtrar por período fiscal</t>
-  </si>
-  <si>
     <t>Deseio la implementacion de la base datos</t>
   </si>
   <si>
@@ -385,15 +382,9 @@
     <t>pruebas del software</t>
   </si>
   <si>
-    <t>deseo facturacion</t>
-  </si>
-  <si>
     <t>deseo control de sucursales</t>
   </si>
   <si>
-    <t>deseo contro de stock</t>
-  </si>
-  <si>
     <t>HU07</t>
   </si>
   <si>
@@ -419,6 +410,18 @@
   </si>
   <si>
     <t>debe emitir los reportes del stock de los diferentes almacenes y manejo de crud</t>
+  </si>
+  <si>
+    <t>deseo emitir boletas de ventas</t>
+  </si>
+  <si>
+    <t>deseo contro de stock de los almacenes</t>
+  </si>
+  <si>
+    <t>Planeado</t>
+  </si>
+  <si>
+    <t>Debe poder mostrar los procesos de las funcionalidades del proceso</t>
   </si>
 </sst>
 </file>
@@ -738,6 +741,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -770,18 +785,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,8 +1365,8 @@
   </sheetPr>
   <dimension ref="B1:S80"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1400,14 +1403,14 @@
       </c>
     </row>
     <row r="2" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="56"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -1426,14 +1429,14 @@
       </c>
     </row>
     <row r="3" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="56"/>
+      <c r="E3" s="60"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -1474,27 +1477,27 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52" t="s">
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="54"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="58"/>
     </row>
     <row r="6" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="34" t="s">
@@ -1586,7 +1589,7 @@
         <v>53</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8" s="8">
         <v>1</v>
@@ -1601,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P8" s="9"/>
     </row>
@@ -1623,7 +1626,7 @@
         <v>53</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K9" s="8">
         <v>1</v>
@@ -1638,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P9" s="9"/>
     </row>
@@ -1660,7 +1663,7 @@
         <v>54</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="K10" s="8">
         <v>1</v>
@@ -1675,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P10" s="9"/>
     </row>
@@ -1716,13 +1719,13 @@
         <v>46</v>
       </c>
       <c r="H12" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K12" s="8">
         <v>1</v>
@@ -1737,7 +1740,7 @@
         <v>4</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P12" s="9"/>
     </row>
@@ -1753,13 +1756,13 @@
         <v>46</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K13" s="8">
         <v>1</v>
@@ -1774,7 +1777,7 @@
         <v>5</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P13" s="9"/>
     </row>
@@ -1790,13 +1793,13 @@
         <v>46</v>
       </c>
       <c r="H14" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K14" s="8">
         <v>1</v>
@@ -1811,7 +1814,7 @@
         <v>6</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P14" s="9"/>
     </row>
@@ -1823,10 +1826,10 @@
         <v>46</v>
       </c>
       <c r="D15" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="42" t="s">
         <v>67</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>68</v>
       </c>
       <c r="F15" s="43"/>
       <c r="G15" s="42"/>
@@ -1846,19 +1849,19 @@
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="42" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G16" s="42" t="s">
         <v>46</v>
       </c>
       <c r="H16" s="42" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="I16" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>75</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>78</v>
       </c>
       <c r="K16" s="8">
         <v>1</v>
@@ -1867,13 +1870,13 @@
         <v>10</v>
       </c>
       <c r="M16" s="45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N16" s="8">
         <v>7</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P16" s="9"/>
     </row>
@@ -1883,19 +1886,19 @@
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
       <c r="F17" s="42" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G17" s="42" t="s">
         <v>46</v>
       </c>
       <c r="H17" s="42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I17" s="42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K17" s="8">
         <v>1</v>
@@ -1904,13 +1907,13 @@
         <v>10</v>
       </c>
       <c r="M17" s="45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N17" s="8">
         <v>8</v>
       </c>
       <c r="O17" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P17" s="9"/>
     </row>
@@ -1920,19 +1923,19 @@
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="42" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G18" s="42" t="s">
         <v>46</v>
       </c>
       <c r="H18" s="42" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="I18" s="42" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K18" s="8">
         <v>1</v>
@@ -1941,13 +1944,13 @@
         <v>10</v>
       </c>
       <c r="M18" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="N18" s="8">
         <v>9</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P18" s="9"/>
     </row>
@@ -2635,7 +2638,7 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2698,7 +2701,7 @@
         <v>30</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="15"/>
@@ -2723,7 +2726,7 @@
         <v>40</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
@@ -2748,7 +2751,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="15"/>
@@ -2773,7 +2776,7 @@
         <v>40</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="15"/>
@@ -2798,7 +2801,7 @@
         <v>40</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="15"/>
@@ -2823,89 +2826,89 @@
         <v>40</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="57">
+      <c r="B9" s="46">
         <v>7</v>
       </c>
-      <c r="C9" s="58">
+      <c r="C9" s="47">
         <f t="shared" ref="C9:C17" si="2">IF(AND(C8&lt;&gt;"",D8&lt;&gt;"",D9&lt;&gt;""),C8+D8,"")</f>
         <v>45048</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="48">
         <v>2</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="49">
         <f t="shared" ref="E9:E17" si="3">IF(AND(C9&lt;&gt;"",D9&lt;&gt;""),C9+D9-1,"")</f>
         <v>45049</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="46">
         <f>IF(B9="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B9,'Backlog del Producto'!L$8:L$130))</f>
         <v>10</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="57">
+      <c r="B10" s="46">
         <v>8</v>
       </c>
-      <c r="C10" s="58">
+      <c r="C10" s="47">
         <f t="shared" si="2"/>
         <v>45050</v>
       </c>
-      <c r="D10" s="59">
+      <c r="D10" s="48">
         <v>2</v>
       </c>
-      <c r="E10" s="60">
+      <c r="E10" s="49">
         <f t="shared" si="3"/>
         <v>45051</v>
       </c>
-      <c r="F10" s="57">
+      <c r="F10" s="46">
         <f>IF(B10="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B10,'Backlog del Producto'!L$8:L$130))</f>
         <v>10</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="15"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="57">
+      <c r="B11" s="46">
         <v>9</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="47">
         <f t="shared" si="2"/>
         <v>45052</v>
       </c>
-      <c r="D11" s="59">
+      <c r="D11" s="48">
         <v>2</v>
       </c>
-      <c r="E11" s="60">
+      <c r="E11" s="49">
         <f t="shared" si="3"/>
         <v>45053</v>
       </c>
-      <c r="F11" s="57">
+      <c r="F11" s="46">
         <f>IF(B11="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B11,'Backlog del Producto'!L$8:L$130))</f>
         <v>10</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="17" t="str">
-        <f t="shared" ref="B9:B17" si="4">IF(AND(C12&lt;&gt;"",D12&lt;&gt;""),B11+1,"")</f>
+        <f t="shared" ref="B12:B17" si="4">IF(AND(C12&lt;&gt;"",D12&lt;&gt;""),B11+1,"")</f>
         <v/>
       </c>
       <c r="C12" s="19" t="str">
@@ -2922,7 +2925,7 @@
         <v/>
       </c>
       <c r="G12" s="18" t="str">
-        <f t="shared" ref="G9:G17" si="5">IF(AND(OR(G11="Planned",G11="Ongoing"),D12&lt;&gt;""),"Planned","Unplanned")</f>
+        <f t="shared" ref="G12:G17" si="5">IF(AND(OR(G11="Planned",G11="Ongoing"),D12&lt;&gt;""),"Planned","Unplanned")</f>
         <v>Unplanned</v>
       </c>
       <c r="H12" s="20"/>
@@ -3109,30 +3112,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3245187f-2b70-4b96-af74-b65b25777eca" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="100486ed-dfc5-4b43-a390-ed80e6fa3473">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ECBD21C84E4C4B48B27A6166FAC051E5" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="bb6739421a50b20a8dee76844e41c5f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="100486ed-dfc5-4b43-a390-ed80e6fa3473" xmlns:ns3="3245187f-2b70-4b96-af74-b65b25777eca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="093860096c687094a446cbcfc6e32844" ns2:_="" ns3:_="">
     <xsd:import namespace="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
@@ -3309,15 +3288,58 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3245187f-2b70-4b96-af74-b65b25777eca" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="100486ed-dfc5-4b43-a390-ed80e6fa3473">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B83DAEE-35DE-44AA-B387-4AFD3E8AB467}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
+    <ds:schemaRef ds:uri="3245187f-2b70-4b96-af74-b65b25777eca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3335,29 +3357,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B83DAEE-35DE-44AA-B387-4AFD3E8AB467}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="100486ed-dfc5-4b43-a390-ed80e6fa3473"/>
-    <ds:schemaRef ds:uri="3245187f-2b70-4b96-af74-b65b25777eca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>